<commit_message>
SU plots Top synthese
</commit_message>
<xml_diff>
--- a/SU_Suspension/00_configurations points LAS/Invictus_3421/ARBdisplacement.xlsx
+++ b/SU_Suspension/00_configurations points LAS/Invictus_3421/ARBdisplacement.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9630"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9630" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="bump" sheetId="2" r:id="rId1"/>
@@ -365,8 +365,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:J14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -759,10 +759,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -792,94 +792,94 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
       <c r="D2">
-        <v>1575</v>
+        <v>1574.9</v>
       </c>
       <c r="E2">
-        <v>226.97</v>
+        <v>214.65</v>
       </c>
       <c r="F2">
-        <v>443.61</v>
+        <v>431.01</v>
       </c>
       <c r="I2">
-        <f>F2-$F$8</f>
-        <v>11.610000000000014</v>
+        <f>F2-$F$7</f>
+        <v>-0.99000000000000909</v>
       </c>
       <c r="J2">
-        <f>(I2-I3)/(A2-A3)</f>
-        <v>0.37400000000000089</v>
+        <f>(I2-I3)/(B2-B3)</f>
+        <v>-0.60000000000002274</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
-        <v>1575</v>
+        <v>1574.9</v>
       </c>
       <c r="E3">
-        <v>227.7</v>
+        <v>217.89</v>
       </c>
       <c r="F3">
-        <v>441.74</v>
+        <v>431.31</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I14" si="0">F3-$F$8</f>
-        <v>9.7400000000000091</v>
+        <f t="shared" ref="I3:I12" si="0">F3-$F$7</f>
+        <v>-0.68999999999999773</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J13" si="1">(I3-I4)/(A3-A4)</f>
-        <v>0.38000000000000683</v>
+        <f t="shared" ref="J3:J12" si="1">(I3-I4)/(B3-B4)</f>
+        <v>-0.48000000000001819</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
       <c r="D4">
-        <v>1575</v>
+        <v>1574.9</v>
       </c>
       <c r="E4">
-        <v>228.3</v>
+        <v>220.97</v>
       </c>
       <c r="F4">
-        <v>439.84</v>
+        <v>431.55</v>
       </c>
       <c r="I4">
         <f t="shared" si="0"/>
-        <v>7.839999999999975</v>
+        <v>-0.44999999999998863</v>
       </c>
       <c r="J4">
         <f t="shared" si="1"/>
-        <v>0.38599999999999002</v>
+        <v>-0.37999999999999545</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -888,26 +888,26 @@
         <v>1575</v>
       </c>
       <c r="E5">
-        <v>228.76</v>
+        <v>223.91</v>
       </c>
       <c r="F5">
-        <v>437.91</v>
+        <v>431.74</v>
       </c>
       <c r="I5">
         <f t="shared" si="0"/>
-        <v>5.910000000000025</v>
+        <v>-0.25999999999999091</v>
       </c>
       <c r="J5">
         <f t="shared" si="1"/>
-        <v>0.39000000000000912</v>
+        <v>-0.29999999999995453</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -916,23 +916,23 @@
         <v>1575</v>
       </c>
       <c r="E6">
-        <v>229.09</v>
+        <v>226.7</v>
       </c>
       <c r="F6">
-        <v>435.96</v>
+        <v>431.89</v>
       </c>
       <c r="I6">
         <f t="shared" si="0"/>
-        <v>3.9599999999999795</v>
+        <v>-0.11000000000001364</v>
       </c>
       <c r="J6">
         <f t="shared" si="1"/>
-        <v>0.39399999999999408</v>
+        <v>-0.22000000000002728</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -944,18 +944,18 @@
         <v>1575</v>
       </c>
       <c r="E7">
-        <v>229.3</v>
+        <v>229.36</v>
       </c>
       <c r="F7">
-        <v>433.99</v>
+        <v>432</v>
       </c>
       <c r="I7">
         <f t="shared" si="0"/>
-        <v>1.9900000000000091</v>
+        <v>0</v>
       </c>
       <c r="J7">
         <f t="shared" si="1"/>
-        <v>0.3980000000000018</v>
+        <v>-0.13999999999998636</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -963,7 +963,7 @@
         <v>0</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -972,26 +972,26 @@
         <v>1575</v>
       </c>
       <c r="E8">
-        <v>229.36</v>
+        <v>231.89</v>
       </c>
       <c r="F8">
-        <v>432</v>
+        <v>432.07</v>
       </c>
       <c r="I8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.9999999999993179E-2</v>
       </c>
       <c r="J8">
         <f t="shared" si="1"/>
-        <v>0.40199999999999819</v>
+        <v>-8.0000000000040927E-2</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -1000,161 +1000,108 @@
         <v>1575</v>
       </c>
       <c r="E9">
-        <v>229.29</v>
+        <v>234.3</v>
       </c>
       <c r="F9">
-        <v>429.99</v>
+        <v>432.11</v>
       </c>
       <c r="I9">
         <f t="shared" si="0"/>
-        <v>-2.0099999999999909</v>
+        <v>0.11000000000001364</v>
       </c>
       <c r="J9">
         <f t="shared" si="1"/>
-        <v>0.40399999999999636</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>-1.5</v>
       </c>
       <c r="C10">
         <v>0</v>
       </c>
       <c r="D10">
-        <v>1575</v>
+        <v>1575.1</v>
       </c>
       <c r="E10">
-        <v>229.09</v>
+        <v>236.57</v>
       </c>
       <c r="F10">
-        <v>427.97</v>
+        <v>432.11</v>
       </c>
       <c r="I10">
         <f t="shared" si="0"/>
-        <v>-4.0299999999999727</v>
+        <v>0.11000000000001364</v>
       </c>
       <c r="J10">
         <f t="shared" si="1"/>
-        <v>0.40800000000000408</v>
+        <v>8.0000000000040927E-2</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="C11">
         <v>0</v>
       </c>
       <c r="D11">
-        <v>1575</v>
+        <v>1575.1</v>
       </c>
       <c r="E11">
-        <v>228.73</v>
+        <v>238.72</v>
       </c>
       <c r="F11">
-        <v>425.93</v>
+        <v>432.07</v>
       </c>
       <c r="I11">
         <f t="shared" si="0"/>
-        <v>-6.0699999999999932</v>
+        <v>6.9999999999993179E-2</v>
       </c>
       <c r="J11">
         <f t="shared" si="1"/>
-        <v>0.41000000000000225</v>
+        <v>0.13999999999998636</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>-20</v>
+        <v>0</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>-2.5</v>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
       <c r="D12">
-        <v>1575</v>
+        <v>1575.1</v>
       </c>
       <c r="E12">
-        <v>228.22</v>
+        <v>240.73</v>
       </c>
       <c r="F12">
-        <v>423.88</v>
+        <v>432</v>
       </c>
       <c r="I12">
         <f t="shared" si="0"/>
-        <v>-8.1200000000000045</v>
+        <v>0</v>
       </c>
       <c r="J12">
         <f t="shared" si="1"/>
-        <v>0.41399999999999865</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>-25</v>
-      </c>
-      <c r="B13">
-        <v>0</v>
-      </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>1575</v>
-      </c>
-      <c r="E13">
-        <v>227.54</v>
-      </c>
-      <c r="F13">
-        <v>421.81</v>
-      </c>
-      <c r="I13">
-        <f t="shared" si="0"/>
-        <v>-10.189999999999998</v>
-      </c>
-      <c r="J13">
-        <f t="shared" si="1"/>
-        <v>0.41799999999999499</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>-30</v>
-      </c>
-      <c r="B14">
-        <v>0</v>
-      </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-      <c r="D14">
-        <v>1575</v>
-      </c>
-      <c r="E14">
-        <v>226.67</v>
-      </c>
-      <c r="F14">
-        <v>419.72</v>
-      </c>
-      <c r="I14">
-        <f t="shared" si="0"/>
-        <v>-12.279999999999973</v>
-      </c>
-      <c r="J14">
-        <f>(I14-I15)/(A14-A15)</f>
-        <v>0.40933333333333244</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A1:F14">
+    <sortCondition descending="1" ref="B1"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
SU plot bump  LAS
</commit_message>
<xml_diff>
--- a/SU_Suspension/00_configurations points LAS/Invictus_3421/ARBdisplacement.xlsx
+++ b/SU_Suspension/00_configurations points LAS/Invictus_3421/ARBdisplacement.xlsx
@@ -363,7 +363,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J34"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I2" sqref="I2:J14"/>
@@ -399,18 +399,18 @@
         <v>1575</v>
       </c>
       <c r="E2">
-        <v>218.81</v>
+        <v>237.18</v>
       </c>
       <c r="F2">
-        <v>444.39</v>
+        <v>452.29</v>
       </c>
       <c r="I2">
-        <f>F2-$F$8</f>
-        <v>12.389999999999986</v>
+        <f t="shared" ref="I2:I14" si="0">F2-$F$8</f>
+        <v>20.29000000000002</v>
       </c>
       <c r="J2">
-        <f>(I2-I3)/(A2-A3)</f>
-        <v>0.4</v>
+        <f t="shared" ref="J2:J14" si="1">(I2-I3)/(A2-A3)</f>
+        <v>0.65600000000000591</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -427,18 +427,18 @@
         <v>1575</v>
       </c>
       <c r="E3">
-        <v>219.59</v>
+        <v>238.46</v>
       </c>
       <c r="F3">
-        <v>442.39</v>
+        <v>449.01</v>
       </c>
       <c r="I3">
-        <f>F3-$F$8</f>
-        <v>10.389999999999986</v>
+        <f t="shared" si="0"/>
+        <v>17.009999999999991</v>
       </c>
       <c r="J3">
-        <f>(I3-I4)/(A3-A4)</f>
-        <v>0.4079999999999927</v>
+        <f t="shared" si="1"/>
+        <v>0.66599999999999682</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -455,18 +455,18 @@
         <v>1575</v>
       </c>
       <c r="E4">
-        <v>220.23</v>
+        <v>239.51</v>
       </c>
       <c r="F4">
-        <v>440.35</v>
+        <v>445.68</v>
       </c>
       <c r="I4">
-        <f>F4-$F$8</f>
-        <v>8.3500000000000227</v>
+        <f t="shared" si="0"/>
+        <v>13.680000000000007</v>
       </c>
       <c r="J4">
-        <f>(I4-I5)/(A4-A5)</f>
-        <v>0.41200000000000048</v>
+        <f t="shared" si="1"/>
+        <v>0.67400000000000093</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -483,18 +483,18 @@
         <v>1575</v>
       </c>
       <c r="E5">
-        <v>220.72</v>
+        <v>240.32</v>
       </c>
       <c r="F5">
-        <v>438.29</v>
+        <v>442.31</v>
       </c>
       <c r="I5">
-        <f>F5-$F$8</f>
-        <v>6.2900000000000205</v>
+        <f t="shared" si="0"/>
+        <v>10.310000000000002</v>
       </c>
       <c r="J5">
-        <f>(I5-I6)/(A5-A6)</f>
-        <v>0.4160000000000082</v>
+        <f t="shared" si="1"/>
+        <v>0.68200000000000505</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -511,18 +511,18 @@
         <v>1575</v>
       </c>
       <c r="E6">
-        <v>221.08</v>
+        <v>240.9</v>
       </c>
       <c r="F6">
-        <v>436.21</v>
+        <v>438.9</v>
       </c>
       <c r="I6">
-        <f>F6-$F$8</f>
-        <v>4.2099999999999795</v>
+        <f t="shared" si="0"/>
+        <v>6.8999999999999773</v>
       </c>
       <c r="J6">
-        <f>(I6-I7)/(A6-A7)</f>
-        <v>0.41999999999999316</v>
+        <f t="shared" si="1"/>
+        <v>0.6879999999999995</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -539,18 +539,18 @@
         <v>1575</v>
       </c>
       <c r="E7">
-        <v>221.29</v>
+        <v>241.25</v>
       </c>
       <c r="F7">
-        <v>434.11</v>
+        <v>435.46</v>
       </c>
       <c r="I7">
-        <f>F7-$F$8</f>
-        <v>2.1100000000000136</v>
+        <f t="shared" si="0"/>
+        <v>3.4599999999999795</v>
       </c>
       <c r="J7">
-        <f>(I7-I8)/(A7-A8)</f>
-        <v>0.42200000000000271</v>
+        <f t="shared" si="1"/>
+        <v>0.69199999999999595</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -567,18 +567,18 @@
         <v>1575</v>
       </c>
       <c r="E8">
-        <v>221.36</v>
+        <v>241.36</v>
       </c>
       <c r="F8">
         <v>432</v>
       </c>
       <c r="I8">
-        <f>F8-$F$8</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J8">
-        <f>(I8-I9)/(A8-A9)</f>
-        <v>0.4259999999999991</v>
+        <f t="shared" si="1"/>
+        <v>0.69600000000000362</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -595,18 +595,18 @@
         <v>1575</v>
       </c>
       <c r="E9">
-        <v>221.29</v>
+        <v>241.24</v>
       </c>
       <c r="F9">
-        <v>429.87</v>
+        <v>428.52</v>
       </c>
       <c r="I9">
-        <f>F9-$F$8</f>
-        <v>-2.1299999999999955</v>
+        <f t="shared" si="0"/>
+        <v>-3.4800000000000182</v>
       </c>
       <c r="J9">
-        <f>(I9-I10)/(A9-A10)</f>
-        <v>0.42799999999999727</v>
+        <f t="shared" si="1"/>
+        <v>0.70199999999999818</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -623,18 +623,18 @@
         <v>1575</v>
       </c>
       <c r="E10">
-        <v>221.07</v>
+        <v>240.89</v>
       </c>
       <c r="F10">
-        <v>427.73</v>
+        <v>425.01</v>
       </c>
       <c r="I10">
-        <f>F10-$F$8</f>
-        <v>-4.2699999999999818</v>
+        <f t="shared" si="0"/>
+        <v>-6.9900000000000091</v>
       </c>
       <c r="J10">
-        <f>(I10-I11)/(A10-A11)</f>
-        <v>0.43000000000000682</v>
+        <f t="shared" si="1"/>
+        <v>0.70399999999999641</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -651,18 +651,18 @@
         <v>1575</v>
       </c>
       <c r="E11">
-        <v>220.7</v>
+        <v>240.28</v>
       </c>
       <c r="F11">
-        <v>425.58</v>
+        <v>421.49</v>
       </c>
       <c r="I11">
-        <f>F11-$F$8</f>
-        <v>-6.4200000000000159</v>
+        <f t="shared" si="0"/>
+        <v>-10.509999999999991</v>
       </c>
       <c r="J11">
-        <f>(I11-I12)/(A11-A12)</f>
-        <v>0.43199999999999361</v>
+        <f t="shared" si="1"/>
+        <v>0.70800000000000407</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -679,18 +679,18 @@
         <v>1575</v>
       </c>
       <c r="E12">
-        <v>220.17</v>
+        <v>239.4</v>
       </c>
       <c r="F12">
-        <v>423.42</v>
+        <v>417.95</v>
       </c>
       <c r="I12">
-        <f>F12-$F$8</f>
-        <v>-8.5799999999999841</v>
+        <f t="shared" si="0"/>
+        <v>-14.050000000000011</v>
       </c>
       <c r="J12">
-        <f>(I12-I13)/(A12-A13)</f>
-        <v>0.43400000000000316</v>
+        <f t="shared" si="1"/>
+        <v>0.71200000000000041</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -707,18 +707,18 @@
         <v>1575</v>
       </c>
       <c r="E13">
-        <v>219.46</v>
+        <v>238.25</v>
       </c>
       <c r="F13">
-        <v>421.25</v>
+        <v>414.39</v>
       </c>
       <c r="I13">
-        <f>F13-$F$8</f>
-        <v>-10.75</v>
+        <f t="shared" si="0"/>
+        <v>-17.610000000000014</v>
       </c>
       <c r="J13">
-        <f>(I13-I14)/(A13-A14)</f>
-        <v>0.43799999999999956</v>
+        <f t="shared" si="1"/>
+        <v>0.71599999999999686</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -735,23 +735,103 @@
         <v>1575</v>
       </c>
       <c r="E14">
-        <v>218.57</v>
+        <v>236.79</v>
       </c>
       <c r="F14">
-        <v>419.06</v>
+        <v>410.81</v>
       </c>
       <c r="I14">
-        <f>F14-$F$8</f>
-        <v>-12.939999999999998</v>
+        <f t="shared" si="0"/>
+        <v>-21.189999999999998</v>
       </c>
       <c r="J14">
-        <f>(I14-I15)/(A14-A15)</f>
-        <v>0.43133333333333324</v>
+        <f t="shared" si="1"/>
+        <v>0.70633333333333326</v>
+      </c>
+    </row>
+    <row r="18" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E18">
+        <v>30</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>1575</v>
+      </c>
+      <c r="I18">
+        <v>237.18</v>
+      </c>
+      <c r="J18">
+        <v>452.29</v>
+      </c>
+    </row>
+    <row r="19" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E19">
+        <v>25</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>1575</v>
+      </c>
+      <c r="I19">
+        <v>238.46</v>
+      </c>
+      <c r="J19">
+        <v>449.01</v>
+      </c>
+    </row>
+    <row r="20" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E20">
+        <v>20</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>1575</v>
+      </c>
+      <c r="I20">
+        <v>239.51</v>
+      </c>
+      <c r="J20">
+        <v>445.68</v>
+      </c>
+    </row>
+    <row r="21" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E21">
+        <v>15</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>1575</v>
+      </c>
+      <c r="I21">
+        <v>240.32</v>
+      </c>
+      <c r="J21">
+        <v>442.31</v>
       </c>
     </row>
     <row r="22" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E22">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="F22">
         <v>0</v>
@@ -763,15 +843,15 @@
         <v>1575</v>
       </c>
       <c r="I22">
-        <v>218.81</v>
+        <v>240.9</v>
       </c>
       <c r="J22">
-        <v>444.39</v>
+        <v>438.9</v>
       </c>
     </row>
     <row r="23" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E23">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="F23">
         <v>0</v>
@@ -783,15 +863,15 @@
         <v>1575</v>
       </c>
       <c r="I23">
-        <v>219.59</v>
+        <v>241.25</v>
       </c>
       <c r="J23">
-        <v>442.39</v>
+        <v>435.46</v>
       </c>
     </row>
     <row r="24" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E24">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="F24">
         <v>0</v>
@@ -803,15 +883,15 @@
         <v>1575</v>
       </c>
       <c r="I24">
-        <v>220.23</v>
+        <v>241.36</v>
       </c>
       <c r="J24">
-        <v>440.35</v>
+        <v>432</v>
       </c>
     </row>
     <row r="25" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E25">
-        <v>15</v>
+        <v>-5</v>
       </c>
       <c r="F25">
         <v>0</v>
@@ -823,15 +903,15 @@
         <v>1575</v>
       </c>
       <c r="I25">
-        <v>220.72</v>
+        <v>241.24</v>
       </c>
       <c r="J25">
-        <v>438.29</v>
+        <v>428.52</v>
       </c>
     </row>
     <row r="26" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E26">
-        <v>10</v>
+        <v>-10</v>
       </c>
       <c r="F26">
         <v>0</v>
@@ -843,15 +923,15 @@
         <v>1575</v>
       </c>
       <c r="I26">
-        <v>221.08</v>
+        <v>240.89</v>
       </c>
       <c r="J26">
-        <v>436.21</v>
+        <v>425.01</v>
       </c>
     </row>
     <row r="27" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E27">
-        <v>5</v>
+        <v>-15</v>
       </c>
       <c r="F27">
         <v>0</v>
@@ -863,15 +943,15 @@
         <v>1575</v>
       </c>
       <c r="I27">
-        <v>221.29</v>
+        <v>240.28</v>
       </c>
       <c r="J27">
-        <v>434.11</v>
+        <v>421.49</v>
       </c>
     </row>
     <row r="28" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E28">
-        <v>0</v>
+        <v>-20</v>
       </c>
       <c r="F28">
         <v>0</v>
@@ -883,15 +963,15 @@
         <v>1575</v>
       </c>
       <c r="I28">
-        <v>221.36</v>
+        <v>239.4</v>
       </c>
       <c r="J28">
-        <v>432</v>
+        <v>417.95</v>
       </c>
     </row>
     <row r="29" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E29">
-        <v>-5</v>
+        <v>-25</v>
       </c>
       <c r="F29">
         <v>0</v>
@@ -903,15 +983,15 @@
         <v>1575</v>
       </c>
       <c r="I29">
-        <v>221.29</v>
+        <v>238.25</v>
       </c>
       <c r="J29">
-        <v>429.87</v>
+        <v>414.39</v>
       </c>
     </row>
     <row r="30" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E30">
-        <v>-10</v>
+        <v>-30</v>
       </c>
       <c r="F30">
         <v>0</v>
@@ -923,95 +1003,15 @@
         <v>1575</v>
       </c>
       <c r="I30">
-        <v>221.07</v>
+        <v>236.79</v>
       </c>
       <c r="J30">
-        <v>427.73</v>
-      </c>
-    </row>
-    <row r="31" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E31">
-        <v>-15</v>
-      </c>
-      <c r="F31">
-        <v>0</v>
-      </c>
-      <c r="G31">
-        <v>0</v>
-      </c>
-      <c r="H31">
-        <v>1575</v>
-      </c>
-      <c r="I31">
-        <v>220.7</v>
-      </c>
-      <c r="J31">
-        <v>425.58</v>
-      </c>
-    </row>
-    <row r="32" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E32">
-        <v>-20</v>
-      </c>
-      <c r="F32">
-        <v>0</v>
-      </c>
-      <c r="G32">
-        <v>0</v>
-      </c>
-      <c r="H32">
-        <v>1575</v>
-      </c>
-      <c r="I32">
-        <v>220.17</v>
-      </c>
-      <c r="J32">
-        <v>423.42</v>
-      </c>
-    </row>
-    <row r="33" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E33">
-        <v>-25</v>
-      </c>
-      <c r="F33">
-        <v>0</v>
-      </c>
-      <c r="G33">
-        <v>0</v>
-      </c>
-      <c r="H33">
-        <v>1575</v>
-      </c>
-      <c r="I33">
-        <v>219.46</v>
-      </c>
-      <c r="J33">
-        <v>421.25</v>
-      </c>
-    </row>
-    <row r="34" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E34">
-        <v>-30</v>
-      </c>
-      <c r="F34">
-        <v>0</v>
-      </c>
-      <c r="G34">
-        <v>0</v>
-      </c>
-      <c r="H34">
-        <v>1575</v>
-      </c>
-      <c r="I34">
-        <v>218.57</v>
-      </c>
-      <c r="J34">
-        <v>419.06</v>
+        <v>410.81</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="E22:J34">
-    <sortCondition descending="1" ref="E22"/>
+  <sortState ref="E18:J30">
+    <sortCondition descending="1" ref="E18"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
SU maj LASauto points BAR
</commit_message>
<xml_diff>
--- a/SU_Suspension/00_configurations points LAS/Invictus_3421/ARBdisplacement.xlsx
+++ b/SU_Suspension/00_configurations points LAS/Invictus_3421/ARBdisplacement.xlsx
@@ -363,10 +363,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J34"/>
+  <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:J14"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -399,18 +399,18 @@
         <v>1575</v>
       </c>
       <c r="E2">
-        <v>218.81</v>
+        <v>220.49</v>
       </c>
       <c r="F2">
-        <v>444.39</v>
+        <v>456.38</v>
       </c>
       <c r="I2">
-        <f>F2-$F$8</f>
-        <v>12.389999999999986</v>
+        <f t="shared" ref="I2:I14" si="0">F2-$F$8</f>
+        <v>4.3799999999999955</v>
       </c>
       <c r="J2">
-        <f>(I2-I3)/(A2-A3)</f>
-        <v>0.4</v>
+        <f t="shared" ref="J2:J14" si="1">(I2-I3)/(A2-A3)</f>
+        <v>0.15</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -427,18 +427,18 @@
         <v>1575</v>
       </c>
       <c r="E3">
-        <v>219.59</v>
+        <v>220.77</v>
       </c>
       <c r="F3">
-        <v>442.39</v>
+        <v>455.63</v>
       </c>
       <c r="I3">
-        <f>F3-$F$8</f>
-        <v>10.389999999999986</v>
+        <f t="shared" si="0"/>
+        <v>3.6299999999999955</v>
       </c>
       <c r="J3">
-        <f>(I3-I4)/(A3-A4)</f>
-        <v>0.4079999999999927</v>
+        <f t="shared" si="1"/>
+        <v>0.14800000000000182</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -455,18 +455,18 @@
         <v>1575</v>
       </c>
       <c r="E4">
-        <v>220.23</v>
+        <v>220.99</v>
       </c>
       <c r="F4">
-        <v>440.35</v>
+        <v>454.89</v>
       </c>
       <c r="I4">
-        <f>F4-$F$8</f>
-        <v>8.3500000000000227</v>
+        <f t="shared" si="0"/>
+        <v>2.8899999999999864</v>
       </c>
       <c r="J4">
-        <f>(I4-I5)/(A4-A5)</f>
-        <v>0.41200000000000048</v>
+        <f t="shared" si="1"/>
+        <v>0.14599999999999227</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -483,18 +483,18 @@
         <v>1575</v>
       </c>
       <c r="E5">
-        <v>220.72</v>
+        <v>221.16</v>
       </c>
       <c r="F5">
-        <v>438.29</v>
+        <v>454.16</v>
       </c>
       <c r="I5">
-        <f>F5-$F$8</f>
-        <v>6.2900000000000205</v>
+        <f t="shared" si="0"/>
+        <v>2.160000000000025</v>
       </c>
       <c r="J5">
-        <f>(I5-I6)/(A5-A6)</f>
-        <v>0.4160000000000082</v>
+        <f t="shared" si="1"/>
+        <v>0.14600000000000363</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -511,18 +511,18 @@
         <v>1575</v>
       </c>
       <c r="E6">
-        <v>221.08</v>
+        <v>221.27</v>
       </c>
       <c r="F6">
-        <v>436.21</v>
+        <v>453.43</v>
       </c>
       <c r="I6">
-        <f>F6-$F$8</f>
-        <v>4.2099999999999795</v>
+        <f t="shared" si="0"/>
+        <v>1.4300000000000068</v>
       </c>
       <c r="J6">
-        <f>(I6-I7)/(A6-A7)</f>
-        <v>0.41999999999999316</v>
+        <f t="shared" si="1"/>
+        <v>0.14400000000000546</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -539,18 +539,18 @@
         <v>1575</v>
       </c>
       <c r="E7">
-        <v>221.29</v>
+        <v>221.34</v>
       </c>
       <c r="F7">
-        <v>434.11</v>
+        <v>452.71</v>
       </c>
       <c r="I7">
-        <f>F7-$F$8</f>
-        <v>2.1100000000000136</v>
+        <f t="shared" si="0"/>
+        <v>0.70999999999997954</v>
       </c>
       <c r="J7">
-        <f>(I7-I8)/(A7-A8)</f>
-        <v>0.42200000000000271</v>
+        <f t="shared" si="1"/>
+        <v>0.14199999999999591</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -570,15 +570,15 @@
         <v>221.36</v>
       </c>
       <c r="F8">
-        <v>432</v>
+        <v>452</v>
       </c>
       <c r="I8">
-        <f>F8-$F$8</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J8">
-        <f>(I8-I9)/(A8-A9)</f>
-        <v>0.4259999999999991</v>
+        <f t="shared" si="1"/>
+        <v>0.13999999999999774</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -595,18 +595,18 @@
         <v>1575</v>
       </c>
       <c r="E9">
-        <v>221.29</v>
+        <v>221.34</v>
       </c>
       <c r="F9">
-        <v>429.87</v>
+        <v>451.3</v>
       </c>
       <c r="I9">
-        <f>F9-$F$8</f>
-        <v>-2.1299999999999955</v>
+        <f t="shared" si="0"/>
+        <v>-0.69999999999998863</v>
       </c>
       <c r="J9">
-        <f>(I9-I10)/(A9-A10)</f>
-        <v>0.42799999999999727</v>
+        <f t="shared" si="1"/>
+        <v>0.13600000000000137</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -623,18 +623,18 @@
         <v>1575</v>
       </c>
       <c r="E10">
-        <v>221.07</v>
+        <v>221.28</v>
       </c>
       <c r="F10">
-        <v>427.73</v>
+        <v>450.62</v>
       </c>
       <c r="I10">
-        <f>F10-$F$8</f>
-        <v>-4.2699999999999818</v>
+        <f t="shared" si="0"/>
+        <v>-1.3799999999999955</v>
       </c>
       <c r="J10">
-        <f>(I10-I11)/(A10-A11)</f>
-        <v>0.43000000000000682</v>
+        <f t="shared" si="1"/>
+        <v>0.13600000000000137</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -651,18 +651,18 @@
         <v>1575</v>
       </c>
       <c r="E11">
-        <v>220.7</v>
+        <v>221.18</v>
       </c>
       <c r="F11">
-        <v>425.58</v>
+        <v>449.94</v>
       </c>
       <c r="I11">
-        <f>F11-$F$8</f>
-        <v>-6.4200000000000159</v>
+        <f t="shared" si="0"/>
+        <v>-2.0600000000000023</v>
       </c>
       <c r="J11">
-        <f>(I11-I12)/(A11-A12)</f>
-        <v>0.43199999999999361</v>
+        <f t="shared" si="1"/>
+        <v>0.132000000000005</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -679,18 +679,18 @@
         <v>1575</v>
       </c>
       <c r="E12">
-        <v>220.17</v>
+        <v>221.03</v>
       </c>
       <c r="F12">
-        <v>423.42</v>
+        <v>449.28</v>
       </c>
       <c r="I12">
-        <f>F12-$F$8</f>
-        <v>-8.5799999999999841</v>
+        <f t="shared" si="0"/>
+        <v>-2.7200000000000273</v>
       </c>
       <c r="J12">
-        <f>(I12-I13)/(A12-A13)</f>
-        <v>0.43400000000000316</v>
+        <f t="shared" si="1"/>
+        <v>0.12799999999999728</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -707,18 +707,18 @@
         <v>1575</v>
       </c>
       <c r="E13">
-        <v>219.46</v>
+        <v>220.85</v>
       </c>
       <c r="F13">
-        <v>421.25</v>
+        <v>448.64</v>
       </c>
       <c r="I13">
-        <f>F13-$F$8</f>
-        <v>-10.75</v>
+        <f t="shared" si="0"/>
+        <v>-3.3600000000000136</v>
       </c>
       <c r="J13">
-        <f>(I13-I14)/(A13-A14)</f>
-        <v>0.43799999999999956</v>
+        <f t="shared" si="1"/>
+        <v>0.12799999999999728</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -735,23 +735,63 @@
         <v>1575</v>
       </c>
       <c r="E14">
-        <v>218.57</v>
+        <v>220.64</v>
       </c>
       <c r="F14">
-        <v>419.06</v>
+        <v>448</v>
       </c>
       <c r="I14">
-        <f>F14-$F$8</f>
-        <v>-12.939999999999998</v>
+        <f t="shared" si="0"/>
+        <v>-4</v>
       </c>
       <c r="J14">
-        <f>(I14-I15)/(A14-A15)</f>
-        <v>0.43133333333333324</v>
+        <f t="shared" si="1"/>
+        <v>0.13333333333333333</v>
+      </c>
+    </row>
+    <row r="20" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E20">
+        <v>30</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>1575</v>
+      </c>
+      <c r="I20">
+        <v>220.49</v>
+      </c>
+      <c r="J20">
+        <v>456.38</v>
+      </c>
+    </row>
+    <row r="21" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E21">
+        <v>25</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>1575</v>
+      </c>
+      <c r="I21">
+        <v>220.77</v>
+      </c>
+      <c r="J21">
+        <v>455.63</v>
       </c>
     </row>
     <row r="22" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E22">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="F22">
         <v>0</v>
@@ -763,15 +803,15 @@
         <v>1575</v>
       </c>
       <c r="I22">
-        <v>218.81</v>
+        <v>220.99</v>
       </c>
       <c r="J22">
-        <v>444.39</v>
+        <v>454.89</v>
       </c>
     </row>
     <row r="23" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E23">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="F23">
         <v>0</v>
@@ -783,15 +823,15 @@
         <v>1575</v>
       </c>
       <c r="I23">
-        <v>219.59</v>
+        <v>221.16</v>
       </c>
       <c r="J23">
-        <v>442.39</v>
+        <v>454.16</v>
       </c>
     </row>
     <row r="24" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E24">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F24">
         <v>0</v>
@@ -803,15 +843,15 @@
         <v>1575</v>
       </c>
       <c r="I24">
-        <v>220.23</v>
+        <v>221.27</v>
       </c>
       <c r="J24">
-        <v>440.35</v>
+        <v>453.43</v>
       </c>
     </row>
     <row r="25" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E25">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="F25">
         <v>0</v>
@@ -823,15 +863,15 @@
         <v>1575</v>
       </c>
       <c r="I25">
-        <v>220.72</v>
+        <v>221.34</v>
       </c>
       <c r="J25">
-        <v>438.29</v>
+        <v>452.71</v>
       </c>
     </row>
     <row r="26" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E26">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F26">
         <v>0</v>
@@ -843,15 +883,15 @@
         <v>1575</v>
       </c>
       <c r="I26">
-        <v>221.08</v>
+        <v>221.36</v>
       </c>
       <c r="J26">
-        <v>436.21</v>
+        <v>452</v>
       </c>
     </row>
     <row r="27" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E27">
-        <v>5</v>
+        <v>-5</v>
       </c>
       <c r="F27">
         <v>0</v>
@@ -863,15 +903,15 @@
         <v>1575</v>
       </c>
       <c r="I27">
-        <v>221.29</v>
+        <v>221.34</v>
       </c>
       <c r="J27">
-        <v>434.11</v>
+        <v>451.3</v>
       </c>
     </row>
     <row r="28" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E28">
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="F28">
         <v>0</v>
@@ -883,15 +923,15 @@
         <v>1575</v>
       </c>
       <c r="I28">
-        <v>221.36</v>
+        <v>221.28</v>
       </c>
       <c r="J28">
-        <v>432</v>
+        <v>450.62</v>
       </c>
     </row>
     <row r="29" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E29">
-        <v>-5</v>
+        <v>-15</v>
       </c>
       <c r="F29">
         <v>0</v>
@@ -903,15 +943,15 @@
         <v>1575</v>
       </c>
       <c r="I29">
-        <v>221.29</v>
+        <v>221.18</v>
       </c>
       <c r="J29">
-        <v>429.87</v>
+        <v>449.94</v>
       </c>
     </row>
     <row r="30" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E30">
-        <v>-10</v>
+        <v>-20</v>
       </c>
       <c r="F30">
         <v>0</v>
@@ -923,15 +963,15 @@
         <v>1575</v>
       </c>
       <c r="I30">
-        <v>221.07</v>
+        <v>221.03</v>
       </c>
       <c r="J30">
-        <v>427.73</v>
+        <v>449.28</v>
       </c>
     </row>
     <row r="31" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E31">
-        <v>-15</v>
+        <v>-25</v>
       </c>
       <c r="F31">
         <v>0</v>
@@ -943,15 +983,15 @@
         <v>1575</v>
       </c>
       <c r="I31">
-        <v>220.7</v>
+        <v>220.85</v>
       </c>
       <c r="J31">
-        <v>425.58</v>
+        <v>448.64</v>
       </c>
     </row>
     <row r="32" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E32">
-        <v>-20</v>
+        <v>-30</v>
       </c>
       <c r="F32">
         <v>0</v>
@@ -963,55 +1003,15 @@
         <v>1575</v>
       </c>
       <c r="I32">
-        <v>220.17</v>
+        <v>220.64</v>
       </c>
       <c r="J32">
-        <v>423.42</v>
-      </c>
-    </row>
-    <row r="33" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E33">
-        <v>-25</v>
-      </c>
-      <c r="F33">
-        <v>0</v>
-      </c>
-      <c r="G33">
-        <v>0</v>
-      </c>
-      <c r="H33">
-        <v>1575</v>
-      </c>
-      <c r="I33">
-        <v>219.46</v>
-      </c>
-      <c r="J33">
-        <v>421.25</v>
-      </c>
-    </row>
-    <row r="34" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E34">
-        <v>-30</v>
-      </c>
-      <c r="F34">
-        <v>0</v>
-      </c>
-      <c r="G34">
-        <v>0</v>
-      </c>
-      <c r="H34">
-        <v>1575</v>
-      </c>
-      <c r="I34">
-        <v>218.57</v>
-      </c>
-      <c r="J34">
-        <v>419.06</v>
+        <v>448</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="E22:J34">
-    <sortCondition descending="1" ref="E22"/>
+  <sortState ref="E20:J32">
+    <sortCondition descending="1" ref="E20"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
SU calcul ARB stiffness
</commit_message>
<xml_diff>
--- a/SU_Suspension/00_configurations points LAS/Invictus_3421/ARBdisplacement.xlsx
+++ b/SU_Suspension/00_configurations points LAS/Invictus_3421/ARBdisplacement.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9630"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9630" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="bump" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="11">
   <si>
     <t>z-z_0</t>
   </si>
@@ -39,20 +39,42 @@
     <t>y</t>
   </si>
   <si>
-    <t>x</t>
-  </si>
-  <si>
     <t>bump</t>
   </si>
   <si>
     <t>roll</t>
+  </si>
+  <si>
+    <t>ARB to rocker</t>
+  </si>
+  <si>
+    <t>rocker axis</t>
+  </si>
+  <si>
+    <t>FRONT</t>
+  </si>
+  <si>
+    <t>REAR</t>
+  </si>
+  <si>
+    <t>Invictus3421_v25</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -61,15 +83,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -77,14 +105,57 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Migliaia" xfId="1" builtinId="3"/>
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -98,6 +169,1236 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="it-IT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="it-IT" baseline="0"/>
+              <a:t>travel &amp; ratio</a:t>
+            </a:r>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="it-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>roll!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>FRONT</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="60000"/>
+                    <a:lumOff val="40000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="it-IT"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>roll!$B$3:$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-1.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-2.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>roll!$H$3:$H$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>-7.8400000000000034</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-6.3100000000000023</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-4.7699999999999818</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-3.1999999999999886</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-1.6200000000000045</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.6399999999999864</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.3200000000000216</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.039999999999992</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.8100000000000023</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8.6299999999999955</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>roll!$A$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>REAR</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="5.9681758530183676E-2"/>
+                  <c:y val="-0.23432013706620006"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="it-IT"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>roll!$B$17:$B$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-1.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-2.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>roll!$H$17:$H$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>-8.0500000000000114</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-6.5099999999999909</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-4.9300000000000068</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-3.3299999999999841</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-1.6800000000000068</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.7099999999999795</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.4699999999999704</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.2600000000000477</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.089999999999975</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8.9499999999999886</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-37891440"/>
+        <c:axId val="-37890896"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-37891440"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-37890896"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-37890896"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-37891440"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="it-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="it-IT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Grafico 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -365,18 +1666,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView topLeftCell="A9" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
         <v>5</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6</v>
       </c>
       <c r="I1" t="s">
         <v>0</v>
@@ -1019,349 +2320,738 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="3"/>
+      <c r="G1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>2.5</v>
+      </c>
+      <c r="C3">
+        <v>242.07</v>
+      </c>
+      <c r="D3">
+        <v>161.06</v>
+      </c>
+      <c r="E3">
+        <v>202.84</v>
+      </c>
+      <c r="F3">
+        <v>168.9</v>
+      </c>
+      <c r="H3">
+        <f>D3-F3</f>
+        <v>-7.8400000000000034</v>
+      </c>
+      <c r="I3">
+        <f>(H3-H4)/(B3-B4)</f>
+        <v>-3.0600000000000023</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>242.81</v>
+      </c>
+      <c r="D4">
+        <v>160.82</v>
+      </c>
+      <c r="E4">
+        <v>203.31</v>
+      </c>
+      <c r="F4">
+        <v>167.13</v>
+      </c>
+      <c r="H4">
+        <f t="shared" ref="H4:H13" si="0">D4-F4</f>
+        <v>-6.3100000000000023</v>
+      </c>
+      <c r="I4">
+        <f>(H4-H5)/(B4-B5)</f>
+        <v>-3.0800000000000409</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>1.5</v>
+      </c>
+      <c r="C5">
+        <v>243.47</v>
+      </c>
+      <c r="D5">
+        <v>160.58000000000001</v>
+      </c>
+      <c r="E5">
+        <v>203.75</v>
+      </c>
+      <c r="F5">
+        <v>165.35</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>-4.7699999999999818</v>
+      </c>
+      <c r="I5">
+        <f>(H5-H6)/(B5-B6)</f>
+        <v>-3.1399999999999864</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>244.06</v>
+      </c>
+      <c r="D6">
+        <v>160.37</v>
+      </c>
+      <c r="E6">
+        <v>204.18</v>
+      </c>
+      <c r="F6">
+        <v>163.57</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>-3.1999999999999886</v>
+      </c>
+      <c r="I6">
+        <f>(H6-H7)/(B6-B7)</f>
+        <v>-3.1599999999999682</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <v>0.5</v>
+      </c>
+      <c r="C7">
+        <v>244.57</v>
+      </c>
+      <c r="D7">
+        <v>160.16999999999999</v>
+      </c>
+      <c r="E7">
+        <v>204.6</v>
+      </c>
+      <c r="F7">
+        <v>161.79</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>-1.6200000000000045</v>
+      </c>
+      <c r="I7">
+        <f>(H7-H8)/(B7-B8)</f>
+        <v>-3.2400000000000091</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>0</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>245</v>
+      </c>
+      <c r="D8">
+        <v>160</v>
+      </c>
+      <c r="E8">
+        <v>205</v>
+      </c>
+      <c r="F8">
+        <v>160</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <f>(H8-H9)/(B8-B9)</f>
+        <v>-3.2799999999999727</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>0</v>
+      </c>
+      <c r="B9">
+        <v>-0.5</v>
+      </c>
+      <c r="C9">
+        <v>245.35</v>
+      </c>
+      <c r="D9">
+        <v>159.85</v>
+      </c>
+      <c r="E9">
+        <v>205.38</v>
+      </c>
+      <c r="F9">
+        <v>158.21</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>1.6399999999999864</v>
+      </c>
+      <c r="I9">
+        <f>(H9-H10)/(B9-B10)</f>
+        <v>-3.3600000000000705</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>0</v>
+      </c>
+      <c r="B10">
+        <v>-1</v>
+      </c>
+      <c r="C10">
+        <v>245.61</v>
+      </c>
+      <c r="D10">
+        <v>159.74</v>
+      </c>
+      <c r="E10">
+        <v>205.75</v>
+      </c>
+      <c r="F10">
+        <v>156.41999999999999</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>3.3200000000000216</v>
+      </c>
+      <c r="I10">
+        <f>(H10-H11)/(B10-B11)</f>
+        <v>-3.4399999999999409</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>0</v>
+      </c>
+      <c r="B11">
+        <v>-1.5</v>
+      </c>
+      <c r="C11">
+        <v>245.79</v>
+      </c>
+      <c r="D11">
+        <v>159.66</v>
+      </c>
+      <c r="E11">
+        <v>206.11</v>
+      </c>
+      <c r="F11">
+        <v>154.62</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>5.039999999999992</v>
+      </c>
+      <c r="I11">
+        <f>(H11-H12)/(B11-B12)</f>
+        <v>-3.5400000000000205</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>0</v>
+      </c>
+      <c r="B12">
+        <v>-2</v>
+      </c>
+      <c r="C12">
+        <v>245.86</v>
+      </c>
+      <c r="D12">
+        <v>159.63</v>
+      </c>
+      <c r="E12">
+        <v>206.44</v>
+      </c>
+      <c r="F12">
+        <v>152.82</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>6.8100000000000023</v>
+      </c>
+      <c r="I12">
+        <f>(H12-H13)/(B12-B13)</f>
+        <v>-3.6399999999999864</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>0</v>
+      </c>
+      <c r="B13">
+        <v>-2.5</v>
+      </c>
+      <c r="C13">
+        <v>245.82</v>
+      </c>
+      <c r="D13">
+        <v>159.65</v>
+      </c>
+      <c r="E13">
+        <v>206.77</v>
+      </c>
+      <c r="F13">
+        <v>151.02000000000001</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="0"/>
+        <v>8.6299999999999955</v>
+      </c>
+      <c r="I13">
+        <f>(H13-H14)/(B13-B14)</f>
+        <v>-3.4519999999999982</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D15" s="3"/>
+      <c r="E15" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" s="3"/>
+      <c r="G15" s="7" t="str">
+        <f>G1</f>
+        <v>Invictus3421_v25</v>
+      </c>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="B16" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="D16" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="I1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="E16" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I16" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>0</v>
+      </c>
+      <c r="B17">
         <v>2.5</v>
       </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>1574.9</v>
-      </c>
-      <c r="E2">
-        <v>214.65</v>
-      </c>
-      <c r="F2">
-        <v>431.01</v>
-      </c>
-      <c r="I2">
-        <f>F2-$F$7</f>
-        <v>-0.99000000000000909</v>
-      </c>
-      <c r="J2">
-        <f>(I2-I3)/(B2-B3)</f>
-        <v>-0.60000000000002274</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>0</v>
-      </c>
-      <c r="B3">
+      <c r="C17">
+        <v>225.62</v>
+      </c>
+      <c r="D17">
+        <v>452.82</v>
+      </c>
+      <c r="E17">
+        <v>196.72</v>
+      </c>
+      <c r="F17">
+        <v>460.87</v>
+      </c>
+      <c r="H17">
+        <f>D17-F17</f>
+        <v>-8.0500000000000114</v>
+      </c>
+      <c r="I17">
+        <f>(H17-H18)/(B17-B18)</f>
+        <v>-3.0800000000000409</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>0</v>
+      </c>
+      <c r="B18">
         <v>2</v>
       </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>1574.9</v>
-      </c>
-      <c r="E3">
-        <v>217.89</v>
-      </c>
-      <c r="F3">
-        <v>431.31</v>
-      </c>
-      <c r="I3">
-        <f t="shared" ref="I3:I12" si="0">F3-$F$7</f>
-        <v>-0.68999999999999773</v>
-      </c>
-      <c r="J3">
-        <f t="shared" ref="J3:J12" si="1">(I3-I4)/(B3-B4)</f>
-        <v>-0.48000000000001819</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>0</v>
-      </c>
-      <c r="B4">
+      <c r="C18">
+        <v>228.69</v>
+      </c>
+      <c r="D18">
+        <v>452.63</v>
+      </c>
+      <c r="E18">
+        <v>199.41</v>
+      </c>
+      <c r="F18">
+        <v>459.14</v>
+      </c>
+      <c r="H18">
+        <f t="shared" ref="H18:H27" si="1">D18-F18</f>
+        <v>-6.5099999999999909</v>
+      </c>
+      <c r="I18">
+        <f>(H18-H19)/(B18-B19)</f>
+        <v>-3.1599999999999682</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>0</v>
+      </c>
+      <c r="B19">
         <v>1.5</v>
       </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>1574.9</v>
-      </c>
-      <c r="E4">
-        <v>220.97</v>
-      </c>
-      <c r="F4">
-        <v>431.55</v>
-      </c>
-      <c r="I4">
-        <f t="shared" si="0"/>
-        <v>-0.44999999999998863</v>
-      </c>
-      <c r="J4">
+      <c r="C19">
+        <v>231.67</v>
+      </c>
+      <c r="D19">
+        <v>452.46</v>
+      </c>
+      <c r="E19">
+        <v>202.08</v>
+      </c>
+      <c r="F19">
+        <v>457.39</v>
+      </c>
+      <c r="H19">
         <f t="shared" si="1"/>
-        <v>-0.37999999999999545</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>0</v>
-      </c>
-      <c r="B5">
+        <v>-4.9300000000000068</v>
+      </c>
+      <c r="I19">
+        <f>(H19-H20)/(B19-B20)</f>
+        <v>-3.2000000000000455</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>0</v>
+      </c>
+      <c r="B20">
         <v>1</v>
       </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>1575</v>
-      </c>
-      <c r="E5">
-        <v>223.91</v>
-      </c>
-      <c r="F5">
-        <v>431.74</v>
-      </c>
-      <c r="I5">
-        <f t="shared" si="0"/>
-        <v>-0.25999999999999091</v>
-      </c>
-      <c r="J5">
+      <c r="C20">
+        <v>234.55</v>
+      </c>
+      <c r="D20">
+        <v>452.29</v>
+      </c>
+      <c r="E20">
+        <v>204.74</v>
+      </c>
+      <c r="F20">
+        <v>455.62</v>
+      </c>
+      <c r="H20">
         <f t="shared" si="1"/>
-        <v>-0.29999999999995453</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>0</v>
-      </c>
-      <c r="B6">
+        <v>-3.3299999999999841</v>
+      </c>
+      <c r="I20">
+        <f>(H20-H21)/(B20-B21)</f>
+        <v>-3.2999999999999545</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>0</v>
+      </c>
+      <c r="B21">
         <v>0.5</v>
       </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>1575</v>
-      </c>
-      <c r="E6">
-        <v>226.7</v>
-      </c>
-      <c r="F6">
-        <v>431.89</v>
-      </c>
-      <c r="I6">
-        <f t="shared" si="0"/>
-        <v>-0.11000000000001364</v>
-      </c>
-      <c r="J6">
+      <c r="C21">
+        <v>237.33</v>
+      </c>
+      <c r="D21">
+        <v>452.14</v>
+      </c>
+      <c r="E21">
+        <v>207.38</v>
+      </c>
+      <c r="F21">
+        <v>453.82</v>
+      </c>
+      <c r="H21">
         <f t="shared" si="1"/>
-        <v>-0.22000000000002728</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>0</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>1575</v>
-      </c>
-      <c r="E7">
-        <v>229.36</v>
-      </c>
-      <c r="F7">
-        <v>432</v>
-      </c>
-      <c r="I7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J7">
+        <v>-1.6800000000000068</v>
+      </c>
+      <c r="I21">
+        <f>(H21-H22)/(B21-B22)</f>
+        <v>-3.3600000000000136</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>0</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>240</v>
+      </c>
+      <c r="D22">
+        <v>452</v>
+      </c>
+      <c r="E22">
+        <v>210</v>
+      </c>
+      <c r="F22">
+        <v>452</v>
+      </c>
+      <c r="H22">
         <f t="shared" si="1"/>
-        <v>-0.13999999999998636</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>0</v>
-      </c>
-      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <f>(H22-H23)/(B22-B23)</f>
+        <v>-3.4199999999999591</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>0</v>
+      </c>
+      <c r="B23">
         <v>-0.5</v>
       </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>1575</v>
-      </c>
-      <c r="E8">
-        <v>231.89</v>
-      </c>
-      <c r="F8">
-        <v>432.07</v>
-      </c>
-      <c r="I8">
-        <f t="shared" si="0"/>
-        <v>6.9999999999993179E-2</v>
-      </c>
-      <c r="J8">
+      <c r="C23">
+        <v>242.56</v>
+      </c>
+      <c r="D23">
+        <v>451.87</v>
+      </c>
+      <c r="E23">
+        <v>212.61</v>
+      </c>
+      <c r="F23">
+        <v>450.16</v>
+      </c>
+      <c r="H23">
         <f t="shared" si="1"/>
-        <v>-8.0000000000040927E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>0</v>
-      </c>
-      <c r="B9">
+        <v>1.7099999999999795</v>
+      </c>
+      <c r="I23">
+        <f>(H23-H24)/(B23-B24)</f>
+        <v>-3.5199999999999818</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>0</v>
+      </c>
+      <c r="B24">
         <v>-1</v>
       </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>1575</v>
-      </c>
-      <c r="E9">
-        <v>234.3</v>
-      </c>
-      <c r="F9">
-        <v>432.11</v>
-      </c>
-      <c r="I9">
-        <f t="shared" si="0"/>
-        <v>0.11000000000001364</v>
-      </c>
-      <c r="J9">
+      <c r="C24">
+        <v>245</v>
+      </c>
+      <c r="D24">
+        <v>451.76</v>
+      </c>
+      <c r="E24">
+        <v>215.2</v>
+      </c>
+      <c r="F24">
+        <v>448.29</v>
+      </c>
+      <c r="H24">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>0</v>
-      </c>
-      <c r="B10">
+        <v>3.4699999999999704</v>
+      </c>
+      <c r="I24">
+        <f>(H24-H25)/(B24-B25)</f>
+        <v>-3.5800000000001546</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>0</v>
+      </c>
+      <c r="B25">
         <v>-1.5</v>
       </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>1575.1</v>
-      </c>
-      <c r="E10">
-        <v>236.57</v>
-      </c>
-      <c r="F10">
-        <v>432.11</v>
-      </c>
-      <c r="I10">
-        <f t="shared" si="0"/>
-        <v>0.11000000000001364</v>
-      </c>
-      <c r="J10">
+      <c r="C25">
+        <v>247.31</v>
+      </c>
+      <c r="D25">
+        <v>451.66</v>
+      </c>
+      <c r="E25">
+        <v>217.78</v>
+      </c>
+      <c r="F25">
+        <v>446.4</v>
+      </c>
+      <c r="H25">
         <f t="shared" si="1"/>
-        <v>8.0000000000040927E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>0</v>
-      </c>
-      <c r="B11">
+        <v>5.2600000000000477</v>
+      </c>
+      <c r="I25">
+        <f>(H25-H26)/(B25-B26)</f>
+        <v>-3.6599999999998545</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>0</v>
+      </c>
+      <c r="B26">
         <v>-2</v>
       </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>1575.1</v>
-      </c>
-      <c r="E11">
-        <v>238.72</v>
-      </c>
-      <c r="F11">
-        <v>432.07</v>
-      </c>
-      <c r="I11">
-        <f t="shared" si="0"/>
-        <v>6.9999999999993179E-2</v>
-      </c>
-      <c r="J11">
+      <c r="C26">
+        <v>249.49</v>
+      </c>
+      <c r="D26">
+        <v>451.58</v>
+      </c>
+      <c r="E26">
+        <v>220.33</v>
+      </c>
+      <c r="F26">
+        <v>444.49</v>
+      </c>
+      <c r="H26">
         <f t="shared" si="1"/>
-        <v>0.13999999999998636</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>0</v>
-      </c>
-      <c r="B12">
+        <v>7.089999999999975</v>
+      </c>
+      <c r="I26">
+        <f>(H26-H27)/(B26-B27)</f>
+        <v>-3.7200000000000273</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>0</v>
+      </c>
+      <c r="B27">
         <v>-2.5</v>
       </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>1575.1</v>
-      </c>
-      <c r="E12">
-        <v>240.73</v>
-      </c>
-      <c r="F12">
-        <v>432</v>
-      </c>
-      <c r="I12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J12">
+      <c r="C27">
+        <v>251.51</v>
+      </c>
+      <c r="D27">
+        <v>451.51</v>
+      </c>
+      <c r="E27">
+        <v>222.88</v>
+      </c>
+      <c r="F27">
+        <v>442.56</v>
+      </c>
+      <c r="H27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>8.9499999999999886</v>
+      </c>
+      <c r="I27">
+        <f>(H27-H28)/(B27-B28)</f>
+        <v>-3.5799999999999956</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A1:F14">
-    <sortCondition descending="1" ref="B1"/>
+  <sortState ref="L20:Q30">
+    <sortCondition descending="1" ref="M20"/>
   </sortState>
+  <mergeCells count="8">
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="G15:I15"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:F15"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
SU maj ARB front
</commit_message>
<xml_diff>
--- a/SU_Suspension/00_configurations points LAS/Invictus_3421/ARBdisplacement.xlsx
+++ b/SU_Suspension/00_configurations points LAS/Invictus_3421/ARBdisplacement.xlsx
@@ -136,21 +136,21 @@
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -385,37 +385,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>-7.8400000000000034</c:v>
+                  <c:v>-15.680000000000007</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-6.3100000000000023</c:v>
+                  <c:v>-12.620000000000005</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-4.7699999999999818</c:v>
+                  <c:v>-9.5399999999999636</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-3.1999999999999886</c:v>
+                  <c:v>-6.3999999999999773</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-1.6200000000000045</c:v>
+                  <c:v>-3.2400000000000091</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.6399999999999864</c:v>
+                  <c:v>3.2799999999999727</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.3200000000000216</c:v>
+                  <c:v>6.6400000000000432</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.039999999999992</c:v>
+                  <c:v>10.079999999999984</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6.8100000000000023</c:v>
+                  <c:v>13.620000000000005</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>8.6299999999999955</c:v>
+                  <c:v>17.259999999999991</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -606,11 +606,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-37891440"/>
-        <c:axId val="-37890896"/>
+        <c:axId val="1444145904"/>
+        <c:axId val="1444144272"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-37891440"/>
+        <c:axId val="1444145904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -667,12 +667,12 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-37890896"/>
+        <c:crossAx val="1444144272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-37890896"/>
+        <c:axId val="1444144272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -729,7 +729,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-37891440"/>
+        <c:crossAx val="1444145904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2320,57 +2320,57 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:P29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N24" sqref="N24"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3" t="s">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3" t="s">
+      <c r="D1" s="7"/>
+      <c r="E1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="6" t="s">
+      <c r="F1" s="7"/>
+      <c r="G1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I2" s="2" t="s">
+      <c r="G2" s="1"/>
+      <c r="H2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2394,12 +2394,12 @@
         <v>168.9</v>
       </c>
       <c r="H3">
-        <f>D3-F3</f>
-        <v>-7.8400000000000034</v>
+        <f>(D3-F3)*2</f>
+        <v>-15.680000000000007</v>
       </c>
       <c r="I3">
-        <f>(H3-H4)/(B3-B4)</f>
-        <v>-3.0600000000000023</v>
+        <f t="shared" ref="I3:I13" si="0">(H3-H4)/(B3-B4)</f>
+        <v>-6.1200000000000045</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -2422,12 +2422,12 @@
         <v>167.13</v>
       </c>
       <c r="H4">
-        <f t="shared" ref="H4:H13" si="0">D4-F4</f>
-        <v>-6.3100000000000023</v>
+        <f t="shared" ref="H4:H13" si="1">(D4-F4)*2</f>
+        <v>-12.620000000000005</v>
       </c>
       <c r="I4">
-        <f>(H4-H5)/(B4-B5)</f>
-        <v>-3.0800000000000409</v>
+        <f t="shared" si="0"/>
+        <v>-6.1600000000000819</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -2450,12 +2450,12 @@
         <v>165.35</v>
       </c>
       <c r="H5">
+        <f t="shared" si="1"/>
+        <v>-9.5399999999999636</v>
+      </c>
+      <c r="I5">
         <f t="shared" si="0"/>
-        <v>-4.7699999999999818</v>
-      </c>
-      <c r="I5">
-        <f>(H5-H6)/(B5-B6)</f>
-        <v>-3.1399999999999864</v>
+        <v>-6.2799999999999727</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -2478,12 +2478,12 @@
         <v>163.57</v>
       </c>
       <c r="H6">
+        <f t="shared" si="1"/>
+        <v>-6.3999999999999773</v>
+      </c>
+      <c r="I6">
         <f t="shared" si="0"/>
-        <v>-3.1999999999999886</v>
-      </c>
-      <c r="I6">
-        <f>(H6-H7)/(B6-B7)</f>
-        <v>-3.1599999999999682</v>
+        <v>-6.3199999999999363</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -2506,12 +2506,12 @@
         <v>161.79</v>
       </c>
       <c r="H7">
+        <f t="shared" si="1"/>
+        <v>-3.2400000000000091</v>
+      </c>
+      <c r="I7">
         <f t="shared" si="0"/>
-        <v>-1.6200000000000045</v>
-      </c>
-      <c r="I7">
-        <f>(H7-H8)/(B7-B8)</f>
-        <v>-3.2400000000000091</v>
+        <v>-6.4800000000000182</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -2534,12 +2534,12 @@
         <v>160</v>
       </c>
       <c r="H8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I8">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <f>(H8-H9)/(B8-B9)</f>
-        <v>-3.2799999999999727</v>
+        <v>-6.5599999999999454</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -2562,12 +2562,12 @@
         <v>158.21</v>
       </c>
       <c r="H9">
+        <f t="shared" si="1"/>
+        <v>3.2799999999999727</v>
+      </c>
+      <c r="I9">
         <f t="shared" si="0"/>
-        <v>1.6399999999999864</v>
-      </c>
-      <c r="I9">
-        <f>(H9-H10)/(B9-B10)</f>
-        <v>-3.3600000000000705</v>
+        <v>-6.720000000000141</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -2590,12 +2590,12 @@
         <v>156.41999999999999</v>
       </c>
       <c r="H10">
+        <f t="shared" si="1"/>
+        <v>6.6400000000000432</v>
+      </c>
+      <c r="I10">
         <f t="shared" si="0"/>
-        <v>3.3200000000000216</v>
-      </c>
-      <c r="I10">
-        <f>(H10-H11)/(B10-B11)</f>
-        <v>-3.4399999999999409</v>
+        <v>-6.8799999999998818</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -2618,12 +2618,12 @@
         <v>154.62</v>
       </c>
       <c r="H11">
+        <f t="shared" si="1"/>
+        <v>10.079999999999984</v>
+      </c>
+      <c r="I11">
         <f t="shared" si="0"/>
-        <v>5.039999999999992</v>
-      </c>
-      <c r="I11">
-        <f>(H11-H12)/(B11-B12)</f>
-        <v>-3.5400000000000205</v>
+        <v>-7.0800000000000409</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -2646,12 +2646,12 @@
         <v>152.82</v>
       </c>
       <c r="H12">
+        <f t="shared" si="1"/>
+        <v>13.620000000000005</v>
+      </c>
+      <c r="I12">
         <f t="shared" si="0"/>
-        <v>6.8100000000000023</v>
-      </c>
-      <c r="I12">
-        <f>(H12-H13)/(B12-B13)</f>
-        <v>-3.6399999999999864</v>
+        <v>-7.2799999999999727</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -2674,62 +2674,62 @@
         <v>151.02000000000001</v>
       </c>
       <c r="H13">
+        <f t="shared" si="1"/>
+        <v>17.259999999999991</v>
+      </c>
+      <c r="I13">
         <f t="shared" si="0"/>
-        <v>8.6299999999999955</v>
-      </c>
-      <c r="I13">
-        <f>(H13-H14)/(B13-B14)</f>
-        <v>-3.4519999999999982</v>
+        <v>-6.9039999999999964</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3" t="s">
+      <c r="B15" s="7"/>
+      <c r="C15" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3" t="s">
+      <c r="D15" s="7"/>
+      <c r="E15" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F15" s="3"/>
-      <c r="G15" s="7" t="str">
+      <c r="F15" s="7"/>
+      <c r="G15" s="5" t="str">
         <f>G1</f>
         <v>Invictus3421_v25</v>
       </c>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="F16" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I16" s="2" t="s">
+      <c r="G16" s="1"/>
+      <c r="H16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I16" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>0</v>
       </c>
@@ -2753,11 +2753,11 @@
         <v>-8.0500000000000114</v>
       </c>
       <c r="I17">
-        <f>(H17-H18)/(B17-B18)</f>
+        <f t="shared" ref="I17:I27" si="2">(H17-H18)/(B17-B18)</f>
         <v>-3.0800000000000409</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>0</v>
       </c>
@@ -2777,15 +2777,15 @@
         <v>459.14</v>
       </c>
       <c r="H18">
-        <f t="shared" ref="H18:H27" si="1">D18-F18</f>
+        <f t="shared" ref="H18:H27" si="3">D18-F18</f>
         <v>-6.5099999999999909</v>
       </c>
       <c r="I18">
-        <f>(H18-H19)/(B18-B19)</f>
+        <f t="shared" si="2"/>
         <v>-3.1599999999999682</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>0</v>
       </c>
@@ -2805,15 +2805,33 @@
         <v>457.39</v>
       </c>
       <c r="H19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>-4.9300000000000068</v>
       </c>
       <c r="I19">
-        <f>(H19-H20)/(B19-B20)</f>
+        <f t="shared" si="2"/>
         <v>-3.2000000000000455</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <v>2.5</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="N19">
+        <v>-7.2885</v>
+      </c>
+      <c r="O19">
+        <v>242.07</v>
+      </c>
+      <c r="P19">
+        <v>161.06</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>0</v>
       </c>
@@ -2833,15 +2851,33 @@
         <v>455.62</v>
       </c>
       <c r="H20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>-3.3299999999999841</v>
       </c>
       <c r="I20">
-        <f>(H20-H21)/(B20-B21)</f>
+        <f t="shared" si="2"/>
         <v>-3.2999999999999545</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <v>2</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <v>-7.2392000000000003</v>
+      </c>
+      <c r="O20">
+        <v>242.81</v>
+      </c>
+      <c r="P20">
+        <v>160.82</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>0</v>
       </c>
@@ -2861,15 +2897,33 @@
         <v>453.82</v>
       </c>
       <c r="H21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>-1.6800000000000068</v>
       </c>
       <c r="I21">
-        <f>(H21-H22)/(B21-B22)</f>
+        <f t="shared" si="2"/>
         <v>-3.3600000000000136</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <v>1.5</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <v>-7.1897000000000002</v>
+      </c>
+      <c r="O21">
+        <v>243.47</v>
+      </c>
+      <c r="P21">
+        <v>160.58000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>0</v>
       </c>
@@ -2889,15 +2943,33 @@
         <v>452</v>
       </c>
       <c r="H22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I22">
-        <f>(H22-H23)/(B22-B23)</f>
+        <f t="shared" si="2"/>
         <v>-3.4199999999999591</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K22">
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <v>1</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
+      <c r="N22">
+        <v>-7.14</v>
+      </c>
+      <c r="O22">
+        <v>244.06</v>
+      </c>
+      <c r="P22">
+        <v>160.37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>0</v>
       </c>
@@ -2917,15 +2989,33 @@
         <v>450.16</v>
       </c>
       <c r="H23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.7099999999999795</v>
       </c>
       <c r="I23">
-        <f>(H23-H24)/(B23-B24)</f>
+        <f t="shared" si="2"/>
         <v>-3.5199999999999818</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <v>0.5</v>
+      </c>
+      <c r="M23">
+        <v>0</v>
+      </c>
+      <c r="N23">
+        <v>-7.0900999999999996</v>
+      </c>
+      <c r="O23">
+        <v>244.57</v>
+      </c>
+      <c r="P23">
+        <v>160.16999999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>0</v>
       </c>
@@ -2945,15 +3035,33 @@
         <v>448.29</v>
       </c>
       <c r="H24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3.4699999999999704</v>
       </c>
       <c r="I24">
-        <f>(H24-H25)/(B24-B25)</f>
+        <f t="shared" si="2"/>
         <v>-3.5800000000001546</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <v>0</v>
+      </c>
+      <c r="N24">
+        <v>-7.04</v>
+      </c>
+      <c r="O24">
+        <v>245</v>
+      </c>
+      <c r="P24">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>0</v>
       </c>
@@ -2973,15 +3081,33 @@
         <v>446.4</v>
       </c>
       <c r="H25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5.2600000000000477</v>
       </c>
       <c r="I25">
-        <f>(H25-H26)/(B25-B26)</f>
+        <f t="shared" si="2"/>
         <v>-3.6599999999998545</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="L25">
+        <v>-0.5</v>
+      </c>
+      <c r="M25">
+        <v>0</v>
+      </c>
+      <c r="N25">
+        <v>-6.9898999999999996</v>
+      </c>
+      <c r="O25">
+        <v>245.35</v>
+      </c>
+      <c r="P25">
+        <v>159.85</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>0</v>
       </c>
@@ -3001,15 +3127,33 @@
         <v>444.49</v>
       </c>
       <c r="H26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7.089999999999975</v>
       </c>
       <c r="I26">
-        <f>(H26-H27)/(B26-B27)</f>
+        <f t="shared" si="2"/>
         <v>-3.7200000000000273</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K26">
+        <v>0</v>
+      </c>
+      <c r="L26">
+        <v>-1</v>
+      </c>
+      <c r="M26">
+        <v>0</v>
+      </c>
+      <c r="N26">
+        <v>-6.9397000000000002</v>
+      </c>
+      <c r="O26">
+        <v>245.61</v>
+      </c>
+      <c r="P26">
+        <v>159.74</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>0</v>
       </c>
@@ -3029,17 +3173,75 @@
         <v>442.56</v>
       </c>
       <c r="H27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>8.9499999999999886</v>
       </c>
       <c r="I27">
-        <f>(H27-H28)/(B27-B28)</f>
+        <f t="shared" si="2"/>
         <v>-3.5799999999999956</v>
       </c>
+      <c r="K27">
+        <v>0</v>
+      </c>
+      <c r="L27">
+        <v>-1.5</v>
+      </c>
+      <c r="M27">
+        <v>0</v>
+      </c>
+      <c r="N27">
+        <v>-6.8895999999999997</v>
+      </c>
+      <c r="O27">
+        <v>245.79</v>
+      </c>
+      <c r="P27">
+        <v>159.66</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K28">
+        <v>0</v>
+      </c>
+      <c r="L28">
+        <v>-2</v>
+      </c>
+      <c r="M28">
+        <v>0</v>
+      </c>
+      <c r="N28">
+        <v>-6.8395000000000001</v>
+      </c>
+      <c r="O28">
+        <v>245.86</v>
+      </c>
+      <c r="P28">
+        <v>159.63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K29">
+        <v>0</v>
+      </c>
+      <c r="L29">
+        <v>-2.5</v>
+      </c>
+      <c r="M29">
+        <v>0</v>
+      </c>
+      <c r="N29">
+        <v>-6.7896999999999998</v>
+      </c>
+      <c r="O29">
+        <v>245.82</v>
+      </c>
+      <c r="P29">
+        <v>159.65</v>
+      </c>
     </row>
   </sheetData>
-  <sortState ref="L20:Q30">
-    <sortCondition descending="1" ref="M20"/>
+  <sortState ref="K19:P29">
+    <sortCondition descending="1" ref="L19"/>
   </sortState>
   <mergeCells count="8">
     <mergeCell ref="G1:I1"/>

</xml_diff>